<commit_message>
Extent Reports unnecessary files deleted
</commit_message>
<xml_diff>
--- a/target/test-classes/testData/Master_Sheet.xlsx
+++ b/target/test-classes/testData/Master_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JuneFrameWork\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80BD8CA-F4A5-4C21-85FD-08949E963D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E5973F-0B38-4275-9CAA-602D288F5A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
   <si>
     <t xml:space="preserve">Sr. No </t>
   </si>
@@ -194,13 +194,16 @@
   </si>
   <si>
     <t>VerifyFlipcartBeautyToyMorePageTest</t>
+  </si>
+  <si>
+    <t>VerifyFlipcartGroceryPageTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,12 +239,6 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2AA198"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -257,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -280,23 +277,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -310,12 +296,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -602,7 +582,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -723,7 +703,7 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -735,7 +715,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -747,7 +727,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -759,7 +739,7 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -768,42 +748,48 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>